<commit_message>
Corrected the VERB_TRIGS.xlsx file by adding Mismatch verbs and codes. Corrected EEGVR_L2_SegmentTool.m to take account of changes of VERB_TRIGS.xlsx.
</commit_message>
<xml_diff>
--- a/VERB_TRIGs.xlsx
+++ b/VERB_TRIGs.xlsx
@@ -1,16 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bolger/matlab/Projects/L2Learning_EEGVR_project/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E291DDC4-08E3-9341-BAA1-72285DD3D6C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17820" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>jeter32.wav</t>
   </si>
@@ -91,13 +103,49 @@
   </si>
   <si>
     <t>slogi32.wav</t>
+  </si>
+  <si>
+    <t>attraperMM.wav</t>
+  </si>
+  <si>
+    <t>caresserMM.wav</t>
+  </si>
+  <si>
+    <t>cognerMM.wav</t>
+  </si>
+  <si>
+    <t>deplacerMM.wav</t>
+  </si>
+  <si>
+    <t>jeterMM.wav</t>
+  </si>
+  <si>
+    <t>lacherMM.wav</t>
+  </si>
+  <si>
+    <t>pivoterMM.wav</t>
+  </si>
+  <si>
+    <t>pousserMM.wav</t>
+  </si>
+  <si>
+    <t>secouerMM.wav</t>
+  </si>
+  <si>
+    <t>souleverMM.wav</t>
+  </si>
+  <si>
+    <t>tapoterMM.wav</t>
+  </si>
+  <si>
+    <t>tomberMM.wav</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -121,6 +169,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -188,8 +242,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -242,6 +297,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -566,16 +629,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -589,7 +658,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -603,7 +672,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -617,7 +686,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -631,7 +700,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -645,7 +714,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -659,7 +728,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -673,7 +742,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -687,7 +756,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -701,7 +770,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -715,7 +784,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -729,7 +798,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -741,6 +810,114 @@
       </c>
       <c r="E12">
         <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <f>B1+100</f>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <f>B2+100</f>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ref="B14:B24" si="0">B3+100</f>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>